<commit_message>
Update furnace parts and materials files
</commit_message>
<xml_diff>
--- a/float_zone_IKZ/Fz_furnace_parts.xlsx
+++ b/float_zone_IKZ/Fz_furnace_parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\brueckner\schemas\AreaA-data_modeling_and_schemas\float_zone_IKZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBF800B-DBD5-4EE8-BFC7-586C783D9A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79134E9-E5DA-4D99-ADED-69AB4646020C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coil" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
   <si>
     <t># start Header</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t># end Header</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>mm</t>
@@ -688,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,7 +735,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
@@ -772,13 +769,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -888,19 +885,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -950,23 +947,21 @@
       <c r="X8" s="5"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="A9" s="11"/>
       <c r="B9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -994,7 +989,7 @@
       <c r="D10" s="8"/>
       <c r="E10" s="18"/>
       <c r="F10" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
@@ -1113,16 +1108,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1209,10 +1204,10 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -1253,22 +1248,22 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="E9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="11"/>
@@ -1438,16 +1433,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1490,10 +1485,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1578,22 +1573,22 @@
     </row>
     <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="11"/>
@@ -1679,16 +1674,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1727,10 +1722,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -1807,22 +1802,22 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="E9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="G9" s="6"/>
       <c r="I9" s="6"/>
@@ -1853,7 +1848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EBF8F9-35F4-4FF9-B0C3-CC2BF2C2EAF1}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
@@ -1890,7 +1885,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -1947,16 +1942,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="E9" s="6"/>
     </row>
@@ -2004,7 +1999,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -2055,16 +2050,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="E9" s="6"/>
     </row>

</xml_diff>